<commit_message>
Edited a duplicate in the spreadsheet
</commit_message>
<xml_diff>
--- a/CBD/Locations.xlsx
+++ b/CBD/Locations.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="259">
   <si>
     <t>Organization</t>
   </si>
@@ -1015,6 +1015,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1281,10 +1329,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1000"/>
+  <dimension ref="A1:F999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.125" defaultRowHeight="15" customHeight="1"/>
@@ -1379,762 +1427,750 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="6">
+        <v>8</v>
+      </c>
+      <c r="F5" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="9">
+        <v>20</v>
+      </c>
+      <c r="F6" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="6">
         <v>19</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="F7" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="9">
+        <v>18</v>
+      </c>
+      <c r="F8" s="9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="6">
+        <v>26</v>
+      </c>
+      <c r="F9" s="6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="9">
+        <v>18</v>
+      </c>
+      <c r="F10" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="6">
+        <v>16</v>
+      </c>
+      <c r="F11" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="9">
+        <v>23</v>
+      </c>
+      <c r="F12" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="6">
         <v>20</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="9" t="s">
+      <c r="F13" s="6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="9">
+        <v>18</v>
+      </c>
+      <c r="F14" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="6">
+        <v>25</v>
+      </c>
+      <c r="F15" s="6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="9">
+        <v>18</v>
+      </c>
+      <c r="F16" s="9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="6">
+        <v>14</v>
+      </c>
+      <c r="F17" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="9">
+        <v>20</v>
+      </c>
+      <c r="F18" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" s="6">
+        <v>19</v>
+      </c>
+      <c r="F19" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" s="9">
+        <v>18</v>
+      </c>
+      <c r="F20" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21" s="6">
+        <v>19</v>
+      </c>
+      <c r="F21" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" s="9">
+        <v>18</v>
+      </c>
+      <c r="F22" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E23" s="6">
+        <v>18</v>
+      </c>
+      <c r="F23" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E24" s="9">
+        <v>14</v>
+      </c>
+      <c r="F24" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E25" s="6">
+        <v>20</v>
+      </c>
+      <c r="F25" s="6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E26" s="9">
+        <v>12</v>
+      </c>
+      <c r="F26" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E27" s="6">
         <v>22</v>
       </c>
-      <c r="E5" s="9">
+      <c r="F27" s="6">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="E28" s="9">
         <v>18</v>
       </c>
-      <c r="F5" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="6">
+      <c r="F28" s="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E29" s="6">
+        <v>18</v>
+      </c>
+      <c r="F29" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="E30" s="9">
+        <v>20</v>
+      </c>
+      <c r="F30" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E31" s="6">
+        <v>19</v>
+      </c>
+      <c r="F31" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E32" s="9">
+        <v>19</v>
+      </c>
+      <c r="F32" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="E34" s="9">
+        <v>13</v>
+      </c>
+      <c r="F34" s="9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="E35" s="6">
+        <v>12</v>
+      </c>
+      <c r="F35" s="6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="E36" s="9">
+        <v>18</v>
+      </c>
+      <c r="F36" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E37" s="6">
+        <v>9</v>
+      </c>
+      <c r="F37" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="E38" s="9">
+        <v>22</v>
+      </c>
+      <c r="F38" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="E39" s="6">
+        <v>19</v>
+      </c>
+      <c r="F39" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="E40" s="9">
+        <v>14</v>
+      </c>
+      <c r="F40" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="E41" s="6">
+        <v>18</v>
+      </c>
+      <c r="F41" s="6">
         <v>8</v>
       </c>
-      <c r="F6" s="6">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="9">
-        <v>20</v>
-      </c>
-      <c r="F7" s="9">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="6">
-        <v>19</v>
-      </c>
-      <c r="F8" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="9">
-        <v>18</v>
-      </c>
-      <c r="F9" s="9">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="6">
-        <v>26</v>
-      </c>
-      <c r="F10" s="6">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="9">
-        <v>18</v>
-      </c>
-      <c r="F11" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" s="6">
-        <v>16</v>
-      </c>
-      <c r="F12" s="6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" s="9">
-        <v>23</v>
-      </c>
-      <c r="F13" s="9">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E14" s="6">
-        <v>20</v>
-      </c>
-      <c r="F14" s="6">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="E15" s="9">
-        <v>18</v>
-      </c>
-      <c r="F15" s="9">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E16" s="6">
-        <v>25</v>
-      </c>
-      <c r="F16" s="6">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="E17" s="9">
-        <v>18</v>
-      </c>
-      <c r="F17" s="9">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E18" s="6">
-        <v>14</v>
-      </c>
-      <c r="F18" s="6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="E19" s="9">
-        <v>20</v>
-      </c>
-      <c r="F19" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="E20" s="6">
-        <v>19</v>
-      </c>
-      <c r="F20" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E21" s="9">
-        <v>18</v>
-      </c>
-      <c r="F21" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E22" s="6">
-        <v>19</v>
-      </c>
-      <c r="F22" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="E23" s="9">
-        <v>18</v>
-      </c>
-      <c r="F23" s="9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E24" s="6">
-        <v>18</v>
-      </c>
-      <c r="F24" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="E25" s="9">
-        <v>14</v>
-      </c>
-      <c r="F25" s="9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="E26" s="6">
-        <v>20</v>
-      </c>
-      <c r="F26" s="6">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="E27" s="9">
-        <v>12</v>
-      </c>
-      <c r="F27" s="9">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="E28" s="6">
-        <v>22</v>
-      </c>
-      <c r="F28" s="6">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="E29" s="9">
-        <v>18</v>
-      </c>
-      <c r="F29" s="9">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="E30" s="6">
-        <v>18</v>
-      </c>
-      <c r="F30" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="E31" s="9">
-        <v>20</v>
-      </c>
-      <c r="F31" s="9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="E32" s="6">
-        <v>19</v>
-      </c>
-      <c r="F32" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="E33" s="9">
-        <v>19</v>
-      </c>
-      <c r="F33" s="9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="E35" s="9">
-        <v>13</v>
-      </c>
-      <c r="F35" s="9">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="E36" s="6">
-        <v>12</v>
-      </c>
-      <c r="F36" s="6">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" s="7" t="s">
-        <v>258</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="D37" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="E37" s="9">
-        <v>18</v>
-      </c>
-      <c r="F37" s="9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
-      <c r="A38" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="E38" s="6">
-        <v>9</v>
-      </c>
-      <c r="F38" s="6">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="E39" s="9">
-        <v>22</v>
-      </c>
-      <c r="F39" s="9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="E40" s="6">
-        <v>19</v>
-      </c>
-      <c r="F40" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="E41" s="9">
-        <v>14</v>
-      </c>
-      <c r="F41" s="9">
-        <v>4</v>
-      </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="E42" s="6">
-        <v>18</v>
-      </c>
-      <c r="F42" s="6">
-        <v>8</v>
-      </c>
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="2"/>
@@ -9791,14 +9827,6 @@
       <c r="D999" s="12"/>
       <c r="E999" s="12"/>
       <c r="F999" s="12"/>
-    </row>
-    <row r="1000" spans="1:6">
-      <c r="A1000" s="2"/>
-      <c r="B1000" s="2"/>
-      <c r="C1000" s="12"/>
-      <c r="D1000" s="12"/>
-      <c r="E1000" s="12"/>
-      <c r="F1000" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>